<commit_message>
David pilot and compilation of all pilots
</commit_message>
<xml_diff>
--- a/FilmFinder/FilmFinder/bin/Release/Subject 10 - xianguo.xlsx
+++ b/FilmFinder/FilmFinder/bin/Release/Subject 10 - xianguo.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Subject 10" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -679,11 +679,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="117818880"/>
-        <c:axId val="117820416"/>
+        <c:axId val="59187584"/>
+        <c:axId val="59190656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117818880"/>
+        <c:axId val="59187584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,7 +692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117820416"/>
+        <c:crossAx val="59190656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -700,7 +700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117820416"/>
+        <c:axId val="59190656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -711,7 +711,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117818880"/>
+        <c:crossAx val="59187584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -970,11 +970,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="132356352"/>
-        <c:axId val="132358144"/>
+        <c:axId val="85892480"/>
+        <c:axId val="92656768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132356352"/>
+        <c:axId val="85892480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132358144"/>
+        <c:crossAx val="92656768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -991,7 +991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132358144"/>
+        <c:axId val="92656768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132356352"/>
+        <c:crossAx val="85892480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1261,11 +1261,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="71600000"/>
-        <c:axId val="71601536"/>
+        <c:axId val="38439936"/>
+        <c:axId val="38449920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71600000"/>
+        <c:axId val="38439936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,7 +1274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71601536"/>
+        <c:crossAx val="38449920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1282,7 +1282,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71601536"/>
+        <c:axId val="38449920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1293,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71600000"/>
+        <c:crossAx val="38439936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1699,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>